<commit_message>
Fixed some THOR related bugs
</commit_message>
<xml_diff>
--- a/data/thor_hov_database.xlsx
+++ b/data/thor_hov_database.xlsx
@@ -19,7 +19,7 @@
     <t>Heat of Vaporization</t>
   </si>
   <si>
-    <t>CASRN</t>
+    <t>CAS Number</t>
   </si>
   <si>
     <t>Name for validation purpose</t>
@@ -6185,12 +6185,12 @@
     </font>
     <font>
       <sz val="8"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="8"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Times New Roman"/>
     </font>
     <font>
@@ -6214,7 +6214,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -6247,13 +6247,13 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6292,13 +6292,13 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6334,46 +6334,46 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6399,7 +6399,7 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -6408,19 +6408,19 @@
     <xf numFmtId="1" fontId="6" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="59" fontId="6" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -6429,28 +6429,28 @@
     <xf numFmtId="2" fontId="6" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="60" fontId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="7" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="61" fontId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="61" fontId="7" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -6471,9 +6471,9 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffa8d08d"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff2b2a29"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff9a9a9a"/>
     </indexedColors>
   </colors>
@@ -6673,12 +6673,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -6711,10 +6711,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -6962,12 +6962,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -7282,10 +7282,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>